<commit_message>
CAMBIOS BOTS Y EJECUCIONES
</commit_message>
<xml_diff>
--- a/bots/documentos/Datos_Contratistas_2024.xlsx
+++ b/bots/documentos/Datos_Contratistas_2024.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SENA\Desktop\bot\documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SENA\Desktop\bot\bots\documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29019BD5-0D95-4049-81B0-905C84206587}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7CF585D-C354-4FD5-B239-0EBDF6463F2E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="274">
   <si>
     <t>Nombre del contratista</t>
   </si>
@@ -886,12 +886,6 @@
   </si>
   <si>
     <t>WILFREDO HERNANDO MORAN GORDILLO</t>
-  </si>
-  <si>
-    <t>Pendiente Por Publicar Oferta</t>
-  </si>
-  <si>
-    <t>PENDIENTE DE CONTRATRAR POR HORAS</t>
   </si>
 </sst>
 </file>
@@ -1356,10 +1350,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F133"/>
+  <dimension ref="A1:F126"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="98" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="A121" zoomScaleNormal="100" zoomScaleSheetLayoutView="98" workbookViewId="0">
+      <selection activeCell="I138" sqref="I138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
@@ -3865,62 +3859,6 @@
         <v>28</v>
       </c>
     </row>
-    <row r="127" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="5" t="s">
-        <v>274</v>
-      </c>
-      <c r="C127" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="128" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="5" t="s">
-        <v>274</v>
-      </c>
-      <c r="C128" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="5" t="s">
-        <v>274</v>
-      </c>
-      <c r="C129" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="5" t="s">
-        <v>274</v>
-      </c>
-      <c r="C130" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="5" t="s">
-        <v>274</v>
-      </c>
-      <c r="C131" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="5" t="s">
-        <v>274</v>
-      </c>
-      <c r="C132" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="5" t="s">
-        <v>275</v>
-      </c>
-      <c r="C133" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="598" r:id="rId1"/>
@@ -3929,28 +3867,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e3ed870e-2cd4-4fcb-abfa-612f6860047f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="eb74a94a-066e-4cfd-8a7e-d8076c8ff863" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010005A3DFDE64F55146A91E7152B25E230E" ma:contentTypeVersion="19" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="71ba2b99c5309eeb5ff4de6ec9c89c37">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="e3ed870e-2cd4-4fcb-abfa-612f6860047f" xmlns:ns3="eb74a94a-066e-4cfd-8a7e-d8076c8ff863" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cef42e6df0e200cb343529819582ce6a" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -4216,27 +4132,29 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC6D1FC1-F2B7-4FD6-A5CD-DA2275163527}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="e3ed870e-2cd4-4fcb-abfa-612f6860047f"/>
-    <ds:schemaRef ds:uri="eb74a94a-066e-4cfd-8a7e-d8076c8ff863"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{85F43C24-8C5B-4E7C-B394-3ED09FC63F74}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e3ed870e-2cd4-4fcb-abfa-612f6860047f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="eb74a94a-066e-4cfd-8a7e-d8076c8ff863" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F939CE5-80F3-4413-95AC-A35424F72DFD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4254,4 +4172,24 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{85F43C24-8C5B-4E7C-B394-3ED09FC63F74}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC6D1FC1-F2B7-4FD6-A5CD-DA2275163527}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="e3ed870e-2cd4-4fcb-abfa-612f6860047f"/>
+    <ds:schemaRef ds:uri="eb74a94a-066e-4cfd-8a7e-d8076c8ff863"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>